<commit_message>
Merged ConnectFour Grid with GUI FXML
</commit_message>
<xml_diff>
--- a/Projektdetails_WS25_Gruppe_1.xlsx
+++ b/Projektdetails_WS25_Gruppe_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Technikum\JavaProjects\quattuor_vincit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AiGN\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768594A9-8826-4D68-BA92-3160E432CF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451FFD86-7145-4BDF-AFD0-722EE57BEE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="149">
   <si>
     <t>Informationen</t>
   </si>
@@ -811,12 +811,6 @@
     <t>Aus einer Liste an anderen UserInnen kann eine/r ausgewählt und eine Spielsession gestartet werden</t>
   </si>
   <si>
-    <t>Aktives Onlinespiel ohne asynchrone Anfrage</t>
-  </si>
-  <si>
-    <t>Spielsessions werden gespeichert und können aus einer Liste ausgewählt werden</t>
-  </si>
-  <si>
     <t>Aktueller Spielstatus kann vom Server abgerufen werden (Asynchron mit Button)</t>
   </si>
   <si>
@@ -852,6 +846,48 @@
   </si>
   <si>
     <t>Git Planung, Projekt Grundstruktur</t>
+  </si>
+  <si>
+    <t>Grundstruktur GUI</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Vanja</t>
+  </si>
+  <si>
+    <t>Gruppenmeeting, Planung, Merging</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Grundstruktur Server-Client TCP</t>
+  </si>
+  <si>
+    <t>Grundstruktur Grid Spiel</t>
+  </si>
+  <si>
+    <t>Laufende Spiele können unterbrochen werden und zu einem anderen Zeitpunkt weiter gespielt werden -&gt; Spielzustand wird sichtbar in einer Liste gespeichert</t>
+  </si>
+  <si>
+    <t>Spieländerungen werden automatisch aktualisiert ohne aktiver Abfrage des Spielers (Checkbox zum Togglen zwischen Automatisches Aktualisieren / Button)</t>
+  </si>
+  <si>
+    <t>Spiellogik / Einzelspieler</t>
+  </si>
+  <si>
+    <t>Aufbau JSON für Abspeichern</t>
+  </si>
+  <si>
+    <t>Server empfang / Datenbank für JSON</t>
+  </si>
+  <si>
+    <t>in Arbeit</t>
   </si>
 </sst>
 </file>
@@ -4607,8 +4643,8 @@
   </sheetPr>
   <dimension ref="B1:C1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4627,7 +4663,7 @@
         <v>55</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="61.5" customHeight="1">
@@ -4635,7 +4671,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="12.75">
@@ -4655,7 +4691,7 @@
     <row r="6" spans="2:3" ht="12.75">
       <c r="B6" s="17"/>
       <c r="C6" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="25.5">
@@ -4663,7 +4699,7 @@
         <v>58</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="25.5">
@@ -4671,7 +4707,7 @@
         <v>59</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="12.75">
@@ -4713,13 +4749,13 @@
     <row r="15" spans="2:3" ht="12.75">
       <c r="B15" s="17"/>
       <c r="C15" s="10" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="12.75">
       <c r="B16" s="17"/>
       <c r="C16" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="12.75">
@@ -4731,19 +4767,19 @@
         <v>62</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="12.75">
       <c r="B19" s="17"/>
       <c r="C19" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="12.75">
       <c r="B20" s="17"/>
       <c r="C20" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="12.75">
@@ -4754,19 +4790,19 @@
         <v>63</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="12.75">
       <c r="B23" s="17"/>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="12.75">
       <c r="B24" s="17"/>
       <c r="C24" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="12.75">
@@ -8698,10 +8734,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:G3"/>
+  <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8738,10 +8774,66 @@
         <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -8754,15 +8846,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:G2"/>
+  <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -8785,6 +8879,39 @@
       </c>
       <c r="G2" s="12" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -8799,7 +8926,9 @@
   </sheetPr>
   <dimension ref="B2:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>

</xml_diff>